<commit_message>
added truncation and commented out the spacy download
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PraxisprojektMaster\inl-meet-ir-v2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BC9FA8A-2B94-4558-8B88-1CE680CC25D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D02532-98A7-4E17-A390-10A5A9753112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="720" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17940" yWindow="3630" windowWidth="14400" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
   <si>
     <t>_id</t>
   </si>
@@ -106,6 +105,15 @@
   <si>
     <t xml:space="preserve">	High_x000D_
 5f86e752316a979c2c3b4d67	Machu Picchu reopened for lone tourist who was stranded in Peru because of COVID-19	This tour is truly amazing, thank you, the grateful tourist said.</t>
+  </si>
+  <si>
+    <t>Lol</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Test Test  Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test  Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test  Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test  Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test  Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test  Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test Test</t>
   </si>
 </sst>
 </file>
@@ -484,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{951CDF9D-C5C6-49A0-A953-C0C3B5A242D7}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,6 +784,20 @@
         <v>26</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>69420</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>